<commit_message>
update impact_items data sheet
</commit_message>
<xml_diff>
--- a/exposan/biogenic_refinery/data/impact_items.xlsx
+++ b/exposan/biogenic_refinery/data/impact_items.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lewisrowles/opt/anaconda3/lib/python3.8/site-packages/exposan/biogenic_refinery/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/opt/anaconda3/lib/python3.8/site-packages/exposan/biogenic_refinery/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324E5037-9B5A-F74D-BEB3-58D598ABC2B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A609FB-09AA-6049-A9C4-FF3D104E0908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5340" yWindow="-17780" windowWidth="27240" windowHeight="16080" activeTab="1" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
+    <workbookView xWindow="980" yWindow="500" windowWidth="27240" windowHeight="15980" activeTab="1" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
@@ -792,7 +792,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1307,13 +1307,13 @@
         <v>22</v>
       </c>
       <c r="C22" s="3">
-        <v>1</v>
+        <v>2.0673798630000002</v>
       </c>
       <c r="D22" s="3">
-        <v>0</v>
+        <v>1.8606418767000001</v>
       </c>
       <c r="E22" s="3">
-        <v>2</v>
+        <v>2.2741178493000005</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>1</v>
@@ -1330,13 +1330,13 @@
         <v>22</v>
       </c>
       <c r="C23" s="3">
-        <v>1</v>
+        <v>1.9299999302999999</v>
       </c>
       <c r="D23" s="3">
-        <v>0</v>
+        <v>1.73699993727</v>
       </c>
       <c r="E23" s="3">
-        <v>2</v>
+        <v>2.1229999233300001</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
add Biogenic Refinery, Eco-San, and Reclaimer
</commit_message>
<xml_diff>
--- a/exposan/biogenic_refinery/data/impact_items.xlsx
+++ b/exposan/biogenic_refinery/data/impact_items.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/opt/anaconda3/lib/python3.8/site-packages/exposan/biogenic_refinery/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hlohm\Dropbox\Lohman-Guest_Shared\12_PhD_Paper3_Sanitation_Decision-Making\Python Code\GitHubDesktop\EXPOsan-private\exposan\biogenic_refinery\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A609FB-09AA-6049-A9C4-FF3D104E0908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5446BFC-7FBE-4E92-93C9-380CD9247ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="500" windowWidth="27240" windowHeight="15980" activeTab="1" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
+    <workbookView xWindow="56085" yWindow="1335" windowWidth="2970" windowHeight="1350" activeTab="4" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
     <sheet name="GWP" sheetId="1" r:id="rId2"/>
+    <sheet name="H_Ecosystems" sheetId="3" r:id="rId3"/>
+    <sheet name="H_Health" sheetId="4" r:id="rId4"/>
+    <sheet name="H_Resources" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="44">
   <si>
     <t>ecoinvent 3</t>
   </si>
@@ -164,6 +167,9 @@
   </si>
   <si>
     <t>Fan</t>
+  </si>
+  <si>
+    <t>points</t>
   </si>
 </sst>
 </file>
@@ -557,16 +563,16 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -574,7 +580,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -582,7 +588,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -590,7 +596,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -598,7 +604,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -606,7 +612,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -614,7 +620,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -622,7 +628,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -630,7 +636,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -638,7 +644,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -646,7 +652,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -654,7 +660,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -662,7 +668,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -670,7 +676,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -678,7 +684,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -686,7 +692,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -694,7 +700,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -702,7 +708,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -710,7 +716,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -718,7 +724,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -726,7 +732,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -734,7 +740,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -742,7 +748,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -750,7 +756,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -758,7 +764,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -766,7 +772,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -774,7 +780,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -791,17 +797,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28627DAA-889C-6942-A3B5-3C8A993554C1}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -824,7 +830,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="str">
         <f>info!A2</f>
         <v>Excavation</v>
@@ -848,7 +854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="str">
         <f>info!A3</f>
         <v>Brick</v>
@@ -872,7 +878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
         <f>info!A4</f>
         <v>Cement</v>
@@ -896,7 +902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
         <f>info!A5</f>
         <v>Concrete</v>
@@ -920,7 +926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
         <f>info!A6</f>
         <v>Gravel</v>
@@ -944,7 +950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="str">
         <f>info!A7</f>
         <v>Plastic</v>
@@ -968,7 +974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="str">
         <f>info!A8</f>
         <v>Sand</v>
@@ -992,7 +998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
         <f>info!A9</f>
         <v>StainlessSteel</v>
@@ -1016,7 +1022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="str">
         <f>info!A10</f>
         <v>StainlessSteelSheet</v>
@@ -1043,7 +1049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
         <f>info!A11</f>
         <v>Steel</v>
@@ -1067,7 +1073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
         <f>info!A12</f>
         <v>Wood</v>
@@ -1091,7 +1097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
         <f>info!A13</f>
         <v>Trucking</v>
@@ -1115,7 +1121,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1138,7 +1144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1161,7 +1167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1184,7 +1190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1207,7 +1213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1230,7 +1236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1253,7 +1259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1276,7 +1282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -1299,7 +1305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -1322,7 +1328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -1345,7 +1351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -1368,7 +1374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1393,7 +1399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1418,7 +1424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1450,4 +1456,2117 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45AFA65E-2AB0-4D0E-8E5A-9EA8A54DBEB2}">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="str">
+        <f>info!A2</f>
+        <v>Excavation</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="5">
+        <v>2.0826975162783804E-3</v>
+      </c>
+      <c r="D2" s="5">
+        <f>C2*0.9</f>
+        <v>1.8744277646505424E-3</v>
+      </c>
+      <c r="E2" s="5">
+        <f>C2*1.1</f>
+        <v>2.2909672679062186E-3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="str">
+        <f>info!A3</f>
+        <v>Brick</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1.25782963589889E-3</v>
+      </c>
+      <c r="D3" s="5">
+        <f t="shared" ref="D3:D27" si="0">C3*0.9</f>
+        <v>1.1320466723090011E-3</v>
+      </c>
+      <c r="E3" s="5">
+        <f t="shared" ref="E3:E27" si="1">C3*1.1</f>
+        <v>1.3836125994887791E-3</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="str">
+        <f>info!A4</f>
+        <v>Cement</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="5">
+        <v>4.2652715832030398E-3</v>
+      </c>
+      <c r="D4" s="5">
+        <f t="shared" si="0"/>
+        <v>3.838744424882736E-3</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" si="1"/>
+        <v>4.6917987415233441E-3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="str">
+        <f>info!A5</f>
+        <v>Concrete</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1.5021122298140999</v>
+      </c>
+      <c r="D5" s="5">
+        <f t="shared" si="0"/>
+        <v>1.35190100683269</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" si="1"/>
+        <v>1.65232345279551</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="str">
+        <f>info!A6</f>
+        <v>Gravel</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="5">
+        <v>8.9239665301849803E-5</v>
+      </c>
+      <c r="D6" s="5">
+        <f t="shared" si="0"/>
+        <v>8.0315698771664818E-5</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" si="1"/>
+        <v>9.8163631832034787E-5</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="str">
+        <f>info!A7</f>
+        <v>Plastic</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="5">
+        <v>7.0545200988693093E-3</v>
+      </c>
+      <c r="D7" s="5">
+        <f t="shared" si="0"/>
+        <v>6.3490680889823781E-3</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="1"/>
+        <v>7.7599721087562405E-3</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="str">
+        <f>info!A8</f>
+        <v>Sand</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="5">
+        <v>5.9466265249932603E-5</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" si="0"/>
+        <v>5.3519638724939347E-5</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="1"/>
+        <v>6.5412891774925866E-5</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="str">
+        <f>info!A9</f>
+        <v>StainlessSteel</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1.8428491258600899E-2</v>
+      </c>
+      <c r="D9" s="5">
+        <f t="shared" si="0"/>
+        <v>1.6585642132740809E-2</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="1"/>
+        <v>2.027134038446099E-2</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="str">
+        <f>info!A10</f>
+        <v>StainlessSteelSheet</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="5">
+        <v>2.6293695623320597E-3</v>
+      </c>
+      <c r="D10" s="5">
+        <f t="shared" si="0"/>
+        <v>2.3664326060988537E-3</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" si="1"/>
+        <v>2.8923065185652661E-3</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="str">
+        <f>info!A11</f>
+        <v>Steel</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="5">
+        <v>8.0947185701723701E-3</v>
+      </c>
+      <c r="D11" s="5">
+        <f t="shared" si="0"/>
+        <v>7.2852467131551335E-3</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" si="1"/>
+        <v>8.9041904271896077E-3</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="str">
+        <f>info!A12</f>
+        <v>Wood</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="5">
+        <v>12.8660077276833</v>
+      </c>
+      <c r="D12" s="5">
+        <f t="shared" si="0"/>
+        <v>11.579406954914971</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="1"/>
+        <v>14.152608500451631</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="str">
+        <f>info!A13</f>
+        <v>Trucking</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="5">
+        <v>7.3491891263938202E-4</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" si="0"/>
+        <v>6.6142702137544386E-4</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="1"/>
+        <v>8.0841080390332029E-4</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0.63456742214387252</v>
+      </c>
+      <c r="D14" s="5">
+        <f t="shared" si="0"/>
+        <v>0.57111067992948528</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" si="1"/>
+        <v>0.69802416435825987</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.30296211312539301</v>
+      </c>
+      <c r="D15" s="5">
+        <f t="shared" si="0"/>
+        <v>0.27266590181285372</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="1"/>
+        <v>0.33325832443793235</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="5">
+        <v>8.0948375438931386</v>
+      </c>
+      <c r="D16" s="5">
+        <f t="shared" si="0"/>
+        <v>7.2853537895038247</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" si="1"/>
+        <v>8.9043212982824524</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1.29272635054464</v>
+      </c>
+      <c r="D17" s="5">
+        <f t="shared" si="0"/>
+        <v>1.1634537154901761</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="1"/>
+        <v>1.4219989855991042</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="5">
+        <v>3.7768807078021105E-2</v>
+      </c>
+      <c r="D18" s="5">
+        <f t="shared" si="0"/>
+        <v>3.3991926370218993E-2</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" si="1"/>
+        <v>4.1545687785823217E-2</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1.29272635054464</v>
+      </c>
+      <c r="D19" s="5">
+        <f t="shared" si="0"/>
+        <v>1.1634537154901761</v>
+      </c>
+      <c r="E19" s="5">
+        <f t="shared" si="1"/>
+        <v>1.4219989855991042</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0.30296211312539301</v>
+      </c>
+      <c r="D20" s="5">
+        <f t="shared" si="0"/>
+        <v>0.27266590181285372</v>
+      </c>
+      <c r="E20" s="5">
+        <f t="shared" si="1"/>
+        <v>0.33325832443793235</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1.9420648277268783E-2</v>
+      </c>
+      <c r="D21" s="5">
+        <f t="shared" si="0"/>
+        <v>1.7478583449541906E-2</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" si="1"/>
+        <v>2.1362713104995663E-2</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="5">
+        <v>7.6122321142258198E-3</v>
+      </c>
+      <c r="D22" s="5">
+        <f t="shared" si="0"/>
+        <v>6.851008902803238E-3</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" si="1"/>
+        <v>8.3734553256484025E-3</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="5">
+        <v>7.0545200988693093E-3</v>
+      </c>
+      <c r="D23" s="5">
+        <f t="shared" si="0"/>
+        <v>6.3490680889823781E-3</v>
+      </c>
+      <c r="E23" s="5">
+        <f t="shared" si="1"/>
+        <v>7.7599721087562405E-3</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="5">
+        <v>3.5277753522681503E-3</v>
+      </c>
+      <c r="D24" s="5">
+        <f t="shared" si="0"/>
+        <v>3.1749978170413353E-3</v>
+      </c>
+      <c r="E24" s="5">
+        <f t="shared" si="1"/>
+        <v>3.8805528874949658E-3</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="5">
+        <v>5.9868875138427702E-3</v>
+      </c>
+      <c r="D25" s="5">
+        <f t="shared" si="0"/>
+        <v>5.3881987624584933E-3</v>
+      </c>
+      <c r="E25" s="5">
+        <f t="shared" si="1"/>
+        <v>6.5855762652270479E-3</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="5">
+        <v>6.9001159923848896E-3</v>
+      </c>
+      <c r="D26" s="5">
+        <f t="shared" si="0"/>
+        <v>6.210104393146401E-3</v>
+      </c>
+      <c r="E26" s="5">
+        <f t="shared" si="1"/>
+        <v>7.5901275916233791E-3</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="5">
+        <v>5.8742658263712E-2</v>
+      </c>
+      <c r="D27" s="5">
+        <f t="shared" si="0"/>
+        <v>5.2868392437340803E-2</v>
+      </c>
+      <c r="E27" s="5">
+        <f t="shared" si="1"/>
+        <v>6.4616924090083211E-2</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{338397C7-E99F-4EAF-BD45-82C00ACD803A}">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="str">
+        <f>info!A2</f>
+        <v>Excavation</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="5">
+        <v>4.0225262172174196E-2</v>
+      </c>
+      <c r="D2" s="5">
+        <f>C2*0.9</f>
+        <v>3.620273595495678E-2</v>
+      </c>
+      <c r="E2" s="5">
+        <f>C2*1.1</f>
+        <v>4.4247788389391619E-2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="str">
+        <f>info!A3</f>
+        <v>Brick</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1.7417474967301703E-2</v>
+      </c>
+      <c r="D3" s="5">
+        <f t="shared" ref="D3:D27" si="0">C3*0.9</f>
+        <v>1.5675727470571534E-2</v>
+      </c>
+      <c r="E3" s="5">
+        <f t="shared" ref="E3:E27" si="1">C3*1.1</f>
+        <v>1.9159222464031875E-2</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="str">
+        <f>info!A4</f>
+        <v>Cement</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="5">
+        <v>5.88741014799046E-2</v>
+      </c>
+      <c r="D4" s="5">
+        <f t="shared" si="0"/>
+        <v>5.2986691331914144E-2</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" si="1"/>
+        <v>6.4761511627895063E-2</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="str">
+        <f>info!A5</f>
+        <v>Concrete</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="5">
+        <v>18.103860435431102</v>
+      </c>
+      <c r="D5" s="5">
+        <f t="shared" si="0"/>
+        <v>16.293474391887994</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" si="1"/>
+        <v>19.914246478974214</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="str">
+        <f>info!A6</f>
+        <v>Gravel</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1.25249603636373E-3</v>
+      </c>
+      <c r="D6" s="5">
+        <f t="shared" si="0"/>
+        <v>1.1272464327273571E-3</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" si="1"/>
+        <v>1.3777456400001031E-3</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="str">
+        <f>info!A7</f>
+        <v>Plastic</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.10059794190115701</v>
+      </c>
+      <c r="D7" s="5">
+        <f t="shared" si="0"/>
+        <v>9.0538147711041309E-2</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="1"/>
+        <v>0.11065773609127272</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="str">
+        <f>info!A8</f>
+        <v>Sand</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="5">
+        <v>8.4207973296428001E-4</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" si="0"/>
+        <v>7.5787175966785197E-4</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="1"/>
+        <v>9.2628770626070804E-4</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="str">
+        <f>info!A9</f>
+        <v>StainlessSteel</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.41384633078614003</v>
+      </c>
+      <c r="D9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.37246169770752602</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="1"/>
+        <v>0.45523096386475409</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="str">
+        <f>info!A10</f>
+        <v>StainlessSteelSheet</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="5">
+        <v>4.9445240467444598E-2</v>
+      </c>
+      <c r="D10" s="5">
+        <f t="shared" si="0"/>
+        <v>4.4500716420700137E-2</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" si="1"/>
+        <v>5.438976451418906E-2</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="str">
+        <f>info!A11</f>
+        <v>Steel</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.15404761894371499</v>
+      </c>
+      <c r="D11" s="5">
+        <f t="shared" si="0"/>
+        <v>0.13864285704934351</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" si="1"/>
+        <v>0.1694523808380865</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="str">
+        <f>info!A12</f>
+        <v>Wood</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="5">
+        <v>7.35373225297442</v>
+      </c>
+      <c r="D12" s="5">
+        <f t="shared" si="0"/>
+        <v>6.6183590276769779</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="1"/>
+        <v>8.089105478271863</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="str">
+        <f>info!A13</f>
+        <v>Trucking</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1.11416240905451E-2</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" si="0"/>
+        <v>1.0027461681490591E-2</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="1"/>
+        <v>1.2255786499599611E-2</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="5">
+        <v>21.804821389423051</v>
+      </c>
+      <c r="D14" s="5">
+        <f t="shared" si="0"/>
+        <v>19.624339250480745</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" si="1"/>
+        <v>23.985303528365357</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="5">
+        <v>14.15675868232</v>
+      </c>
+      <c r="D15" s="5">
+        <f t="shared" si="0"/>
+        <v>12.741082814087999</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="1"/>
+        <v>15.572434550552002</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="5">
+        <v>491.24234300213101</v>
+      </c>
+      <c r="D16" s="5">
+        <f t="shared" si="0"/>
+        <v>442.11810870191789</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" si="1"/>
+        <v>540.36657730234413</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="5">
+        <v>28.560560635650297</v>
+      </c>
+      <c r="D17" s="5">
+        <f t="shared" si="0"/>
+        <v>25.70450457208527</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="1"/>
+        <v>31.416616699215329</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1.7685792692325302</v>
+      </c>
+      <c r="D18" s="5">
+        <f t="shared" si="0"/>
+        <v>1.5917213423092771</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" si="1"/>
+        <v>1.9454371961557833</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="5">
+        <v>28.560560635650297</v>
+      </c>
+      <c r="D19" s="5">
+        <f t="shared" si="0"/>
+        <v>25.70450457208527</v>
+      </c>
+      <c r="E19" s="5">
+        <f t="shared" si="1"/>
+        <v>31.416616699215329</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="5">
+        <v>14.15675868232</v>
+      </c>
+      <c r="D20" s="5">
+        <f t="shared" si="0"/>
+        <v>12.741082814087999</v>
+      </c>
+      <c r="E20" s="5">
+        <f t="shared" si="1"/>
+        <v>15.572434550552002</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0.90748453091794867</v>
+      </c>
+      <c r="D21" s="5">
+        <f t="shared" si="0"/>
+        <v>0.81673607782615387</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" si="1"/>
+        <v>0.99823298400974358</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="5">
+        <v>0.11048229451496501</v>
+      </c>
+      <c r="D22" s="5">
+        <f t="shared" si="0"/>
+        <v>9.943406506346851E-2</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" si="1"/>
+        <v>0.12153052396646152</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="5">
+        <v>0.10059794190115701</v>
+      </c>
+      <c r="D23" s="5">
+        <f t="shared" si="0"/>
+        <v>9.0538147711041309E-2</v>
+      </c>
+      <c r="E23" s="5">
+        <f t="shared" si="1"/>
+        <v>0.11065773609127272</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="5">
+        <v>5.4782882354340402E-2</v>
+      </c>
+      <c r="D24" s="5">
+        <f t="shared" si="0"/>
+        <v>4.9304594118906364E-2</v>
+      </c>
+      <c r="E24" s="5">
+        <f t="shared" si="1"/>
+        <v>6.0261170589774447E-2</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="5">
+        <v>9.4225662775552901E-2</v>
+      </c>
+      <c r="D25" s="5">
+        <f t="shared" si="0"/>
+        <v>8.480309649799761E-2</v>
+      </c>
+      <c r="E25" s="5">
+        <f t="shared" si="1"/>
+        <v>0.10364822905310821</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="5">
+        <v>0.16964282534316702</v>
+      </c>
+      <c r="D26" s="5">
+        <f t="shared" si="0"/>
+        <v>0.15267854280885032</v>
+      </c>
+      <c r="E26" s="5">
+        <f t="shared" si="1"/>
+        <v>0.18660710787748375</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="5">
+        <v>1.88032079219059</v>
+      </c>
+      <c r="D27" s="5">
+        <f t="shared" si="0"/>
+        <v>1.6922887129715309</v>
+      </c>
+      <c r="E27" s="5">
+        <f t="shared" si="1"/>
+        <v>2.0683528714096493</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA7D3C9-542A-47E5-A276-0B7825A720DE}">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="str">
+        <f>info!A2</f>
+        <v>Excavation</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="5">
+        <v>2.73188377175855E-2</v>
+      </c>
+      <c r="D2" s="5">
+        <f>C2*0.9</f>
+        <v>2.458695394582695E-2</v>
+      </c>
+      <c r="E2" s="5">
+        <f>C2*1.1</f>
+        <v>3.0050721489344054E-2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="str">
+        <f>info!A3</f>
+        <v>Brick</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1.10687485072802E-2</v>
+      </c>
+      <c r="D3" s="5">
+        <f t="shared" ref="D3:D27" si="0">C3*0.9</f>
+        <v>9.9618736565521802E-3</v>
+      </c>
+      <c r="E3" s="5">
+        <f t="shared" ref="E3:E27" si="1">C3*1.1</f>
+        <v>1.2175623358008222E-2</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="str">
+        <f>info!A4</f>
+        <v>Cement</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1.5272926695142202E-2</v>
+      </c>
+      <c r="D4" s="5">
+        <f t="shared" si="0"/>
+        <v>1.3745634025627982E-2</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" si="1"/>
+        <v>1.6800219364656425E-2</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="str">
+        <f>info!A5</f>
+        <v>Concrete</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="5">
+        <v>6.9886923389555697</v>
+      </c>
+      <c r="D5" s="5">
+        <f t="shared" si="0"/>
+        <v>6.2898231050600133</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" si="1"/>
+        <v>7.6875615728511271</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="str">
+        <f>info!A6</f>
+        <v>Gravel</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="5">
+        <v>8.3282261971689704E-4</v>
+      </c>
+      <c r="D6" s="5">
+        <f t="shared" si="0"/>
+        <v>7.495403577452073E-4</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" si="1"/>
+        <v>9.1610488168858677E-4</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="str">
+        <f>info!A7</f>
+        <v>Plastic</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.21881932904488599</v>
+      </c>
+      <c r="D7" s="5">
+        <f t="shared" si="0"/>
+        <v>0.1969373961403974</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="1"/>
+        <v>0.24070126194937461</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="str">
+        <f>info!A8</f>
+        <v>Sand</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="5">
+        <v>5.8128590587309102E-4</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" si="0"/>
+        <v>5.2315731528578197E-4</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="1"/>
+        <v>6.3941449646040018E-4</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="str">
+        <f>info!A9</f>
+        <v>StainlessSteel</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.93270074871298803</v>
+      </c>
+      <c r="D9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.83943067384168923</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="1"/>
+        <v>1.0259708235842868</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="str">
+        <f>info!A10</f>
+        <v>StainlessSteelSheet</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="5">
+        <v>6.4849012917126497E-2</v>
+      </c>
+      <c r="D10" s="5">
+        <f t="shared" si="0"/>
+        <v>5.8364111625413849E-2</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" si="1"/>
+        <v>7.1333914208839153E-2</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="str">
+        <f>info!A11</f>
+        <v>Steel</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.12487359988130201</v>
+      </c>
+      <c r="D11" s="5">
+        <f t="shared" si="0"/>
+        <v>0.11238623989317181</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" si="1"/>
+        <v>0.13736095986943223</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="str">
+        <f>info!A12</f>
+        <v>Wood</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="5">
+        <v>5.3991983552999194</v>
+      </c>
+      <c r="D12" s="5">
+        <f t="shared" si="0"/>
+        <v>4.8592785197699273</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="1"/>
+        <v>5.9391181908299115</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="str">
+        <f>info!A13</f>
+        <v>Trucking</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="5">
+        <v>8.5846487710015597E-3</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" si="0"/>
+        <v>7.7261838939014036E-3</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="1"/>
+        <v>9.4431136481017159E-3</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="5">
+        <v>16.1703143438532</v>
+      </c>
+      <c r="D14" s="5">
+        <f t="shared" si="0"/>
+        <v>14.55328290946788</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" si="1"/>
+        <v>17.787345778238521</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="5">
+        <v>8.3066274332224399</v>
+      </c>
+      <c r="D15" s="5">
+        <f t="shared" si="0"/>
+        <v>7.4759646899001959</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="1"/>
+        <v>9.1372901765446848</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="5">
+        <v>536.01328329364594</v>
+      </c>
+      <c r="D16" s="5">
+        <f t="shared" si="0"/>
+        <v>482.41195496428134</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" si="1"/>
+        <v>589.61461162301055</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="5">
+        <v>19.2437545752842</v>
+      </c>
+      <c r="D17" s="5">
+        <f t="shared" si="0"/>
+        <v>17.31937911775578</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="1"/>
+        <v>21.16813003281262</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1.8125326309897301</v>
+      </c>
+      <c r="D18" s="5">
+        <f t="shared" si="0"/>
+        <v>1.6312793678907571</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" si="1"/>
+        <v>1.9937858940887032</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="5">
+        <v>19.2437545752842</v>
+      </c>
+      <c r="D19" s="5">
+        <f t="shared" si="0"/>
+        <v>17.31937911775578</v>
+      </c>
+      <c r="E19" s="5">
+        <f t="shared" si="1"/>
+        <v>21.16813003281262</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="5">
+        <v>8.3066274332224399</v>
+      </c>
+      <c r="D20" s="5">
+        <f t="shared" si="0"/>
+        <v>7.4759646899001959</v>
+      </c>
+      <c r="E20" s="5">
+        <f t="shared" si="1"/>
+        <v>9.1372901765446848</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0.53247611751425894</v>
+      </c>
+      <c r="D21" s="5">
+        <f t="shared" si="0"/>
+        <v>0.47922850576283305</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" si="1"/>
+        <v>0.58572372926568483</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="5">
+        <v>0.150807596748742</v>
+      </c>
+      <c r="D22" s="5">
+        <f t="shared" si="0"/>
+        <v>0.13572683707386782</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" si="1"/>
+        <v>0.16588835642361621</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="5">
+        <v>0.21881932904488599</v>
+      </c>
+      <c r="D23" s="5">
+        <f t="shared" si="0"/>
+        <v>0.1969373961403974</v>
+      </c>
+      <c r="E23" s="5">
+        <f t="shared" si="1"/>
+        <v>0.24070126194937461</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="5">
+        <v>2.9951118606991498E-2</v>
+      </c>
+      <c r="D24" s="5">
+        <f t="shared" si="0"/>
+        <v>2.6956006746292348E-2</v>
+      </c>
+      <c r="E24" s="5">
+        <f t="shared" si="1"/>
+        <v>3.294623046769065E-2</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0.10789022806760601</v>
+      </c>
+      <c r="D25" s="5">
+        <f t="shared" si="0"/>
+        <v>9.7101205260845411E-2</v>
+      </c>
+      <c r="E25" s="5">
+        <f t="shared" si="1"/>
+        <v>0.11867925087436662</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="5">
+        <v>7.7577446363450597E-2</v>
+      </c>
+      <c r="D26" s="5">
+        <f t="shared" si="0"/>
+        <v>6.981970172710554E-2</v>
+      </c>
+      <c r="E26" s="5">
+        <f t="shared" si="1"/>
+        <v>8.5335190999795668E-2</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="5">
+        <v>1.9012293748498701</v>
+      </c>
+      <c r="D27" s="5">
+        <f t="shared" si="0"/>
+        <v>1.7111064373648832</v>
+      </c>
+      <c r="E27" s="5">
+        <f t="shared" si="1"/>
+        <v>2.0913523123348572</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update unit of measure for impact item `Fan`, update pytest setting
</commit_message>
<xml_diff>
--- a/exposan/biogenic_refinery/data/impact_items.xlsx
+++ b/exposan/biogenic_refinery/data/impact_items.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hlohm\Dropbox\Lohman-Guest_Shared\12_PhD_Paper3_Sanitation_Decision-Making\Python Code\GitHubDesktop\EXPOsan-private\exposan\biogenic_refinery\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yalinli_cabbi/Code/EXPOsan/exposan/biogenic_refinery/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5446BFC-7FBE-4E92-93C9-380CD9247ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92893B2F-98CF-4A41-924E-2667FF7BADDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="56085" yWindow="1335" windowWidth="2970" windowHeight="1350" activeTab="4" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
+    <workbookView xWindow="1920" yWindow="4900" windowWidth="38400" windowHeight="21600" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
@@ -562,17 +562,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66379A7A-E84B-1346-816F-577916F7D6A6}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -580,7 +580,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -588,7 +588,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -596,7 +596,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -604,7 +604,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -612,7 +612,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -620,7 +620,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -628,7 +628,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -636,7 +636,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -644,7 +644,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -652,7 +652,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -660,7 +660,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -668,7 +668,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -676,7 +676,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -684,7 +684,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -692,7 +692,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -700,7 +700,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -708,7 +708,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -716,7 +716,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -724,7 +724,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -732,7 +732,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -740,7 +740,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -748,7 +748,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -756,7 +756,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -764,7 +764,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -772,7 +772,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -780,12 +780,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>42</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -801,13 +801,13 @@
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -830,7 +830,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>info!A2</f>
         <v>Excavation</v>
@@ -854,7 +854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>info!A3</f>
         <v>Brick</v>
@@ -878,7 +878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>info!A4</f>
         <v>Cement</v>
@@ -902,7 +902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f>info!A5</f>
         <v>Concrete</v>
@@ -926,7 +926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>info!A6</f>
         <v>Gravel</v>
@@ -950,7 +950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f>info!A7</f>
         <v>Plastic</v>
@@ -974,7 +974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f>info!A8</f>
         <v>Sand</v>
@@ -998,7 +998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
         <f>info!A9</f>
         <v>StainlessSteel</v>
@@ -1022,7 +1022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f>info!A10</f>
         <v>StainlessSteelSheet</v>
@@ -1049,7 +1049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
         <f>info!A11</f>
         <v>Steel</v>
@@ -1073,7 +1073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
         <f>info!A12</f>
         <v>Wood</v>
@@ -1097,7 +1097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
         <f>info!A13</f>
         <v>Trucking</v>
@@ -1121,7 +1121,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1466,13 +1466,13 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>info!A2</f>
         <v>Excavation</v>
@@ -1521,7 +1521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>info!A3</f>
         <v>Brick</v>
@@ -1547,7 +1547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>info!A4</f>
         <v>Cement</v>
@@ -1573,7 +1573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f>info!A5</f>
         <v>Concrete</v>
@@ -1599,7 +1599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>info!A6</f>
         <v>Gravel</v>
@@ -1625,7 +1625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f>info!A7</f>
         <v>Plastic</v>
@@ -1651,7 +1651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f>info!A8</f>
         <v>Sand</v>
@@ -1677,7 +1677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
         <f>info!A9</f>
         <v>StainlessSteel</v>
@@ -1703,7 +1703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f>info!A10</f>
         <v>StainlessSteelSheet</v>
@@ -1729,7 +1729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
         <f>info!A11</f>
         <v>Steel</v>
@@ -1755,7 +1755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
         <f>info!A12</f>
         <v>Wood</v>
@@ -1781,7 +1781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
         <f>info!A13</f>
         <v>Trucking</v>
@@ -1807,7 +1807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -2107,7 +2107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -2171,13 +2171,13 @@
       <selection activeCell="G2" sqref="G2:G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>info!A2</f>
         <v>Excavation</v>
@@ -2226,7 +2226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>info!A3</f>
         <v>Brick</v>
@@ -2252,7 +2252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>info!A4</f>
         <v>Cement</v>
@@ -2278,7 +2278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f>info!A5</f>
         <v>Concrete</v>
@@ -2304,7 +2304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>info!A6</f>
         <v>Gravel</v>
@@ -2330,7 +2330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f>info!A7</f>
         <v>Plastic</v>
@@ -2356,7 +2356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f>info!A8</f>
         <v>Sand</v>
@@ -2382,7 +2382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
         <f>info!A9</f>
         <v>StainlessSteel</v>
@@ -2408,7 +2408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f>info!A10</f>
         <v>StainlessSteelSheet</v>
@@ -2434,7 +2434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
         <f>info!A11</f>
         <v>Steel</v>
@@ -2460,7 +2460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
         <f>info!A12</f>
         <v>Wood</v>
@@ -2486,7 +2486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
         <f>info!A13</f>
         <v>Trucking</v>
@@ -2512,7 +2512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -2587,7 +2587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -2762,7 +2762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -2787,7 +2787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -2812,7 +2812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -2871,17 +2871,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA7D3C9-542A-47E5-A276-0B7825A720DE}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>info!A2</f>
         <v>Excavation</v>
@@ -2930,7 +2930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>info!A3</f>
         <v>Brick</v>
@@ -2956,7 +2956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>info!A4</f>
         <v>Cement</v>
@@ -2982,7 +2982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f>info!A5</f>
         <v>Concrete</v>
@@ -3008,7 +3008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>info!A6</f>
         <v>Gravel</v>
@@ -3034,7 +3034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f>info!A7</f>
         <v>Plastic</v>
@@ -3060,7 +3060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f>info!A8</f>
         <v>Sand</v>
@@ -3086,7 +3086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
         <f>info!A9</f>
         <v>StainlessSteel</v>
@@ -3112,7 +3112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f>info!A10</f>
         <v>StainlessSteelSheet</v>
@@ -3138,7 +3138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
         <f>info!A11</f>
         <v>Steel</v>
@@ -3164,7 +3164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
         <f>info!A12</f>
         <v>Wood</v>
@@ -3190,7 +3190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
         <f>info!A13</f>
         <v>Trucking</v>
@@ -3216,7 +3216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -3266,7 +3266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -3316,7 +3316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -3341,7 +3341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -3366,7 +3366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -3416,7 +3416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -3441,7 +3441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -3541,7 +3541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>42</v>
       </c>

</xml_diff>